<commit_message>
Created Cross-Validation_Performance_Table through SVMWLK. Created new Rmd file for completing Validation and fine tuning of "Building A Model That Helps Locating Displaced People". Archived results in images.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Cross-Validation_Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Cross-Validation_Performance_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77621A5-A8D7-4BCB-8936-A87FA9F748AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794E7E66-CA02-4218-BDEC-0717C4DB1964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="408" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16270" yWindow="50" windowWidth="22000" windowHeight="20850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>LDA</t>
   </si>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>Method Of Determination</t>
-  </si>
-  <si>
-    <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>Logistic Ridge Regression</t>
   </si>
   <si>
     <t>optimal lambda</t>
@@ -124,6 +118,15 @@
   <si>
     <t>cost in excerpt of sequence provided by Peter Gedeck
 corresponding to maximum F1 measure</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>LRR</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +453,48 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC6600"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -613,7 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -628,6 +673,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -675,6 +729,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -983,23 +1042,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1007,10 +1065,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -1022,18 +1080,18 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7">
         <v>0.25</v>
@@ -1057,7 +1115,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1086,12 +1144,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1115,12 +1173,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -1144,12 +1202,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1173,12 +1231,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1202,12 +1260,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1231,236 +1289,291 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>0.98380000000000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="11">
         <v>0.98219999999999996</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="14">
         <v>0.90449999999999997</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="12">
         <v>0.95850000000000002</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="13">
         <v>0.94850000000000001</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="8">
         <v>0.98629999999999995</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="9">
         <v>0.98419999999999996</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="8">
         <v>0.99919999999999998</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="9">
         <v>0.99919999999999998</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="14">
         <v>0.94940000000000002</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="12">
         <v>0.98470000000000002</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="13">
         <v>0.97719999999999996</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="11">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="10">
         <v>0.99850000000000005</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.99590000000000001</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.996</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.99370000000000003</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.99639999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.81120000000000003</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.88770000000000004</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.94550000000000001</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.9698</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.97030000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.99590000000000001</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.996</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.99370000000000003</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.99470000000000003</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.99650000000000005</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.99719999999999998</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.99639999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.8E-3</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1.8E-3</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J14" s="14">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.94110000000000005</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.81120000000000003</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.88770000000000004</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.94550000000000001</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.9698</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0.97030000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0.94330000000000003</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.94450000000000001</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.92149999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2.3E-3</v>
-      </c>
-      <c r="E14" s="3">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="F14" s="3">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1.8E-3</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1.8E-3</v>
-      </c>
-      <c r="I14" s="3">
-        <v>1.9E-3</v>
-      </c>
-      <c r="J14" s="3">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.93010000000000004</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.92869999999999997</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.99109999999999998</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.94330000000000003</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.94640000000000002</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.94450000000000001</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.92149999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.9355</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.89159999999999995</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.94569999999999999</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.95689999999999997</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.94520000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.9355</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.89159999999999995</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.91449999999999998</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.94569999999999999</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.95689999999999997</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.94520000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
       <c r="D17" s="5">
-        <v>-1</v>
+        <f>1*7+1*5+5*3</f>
+        <v>27</v>
       </c>
       <c r="E17" s="5">
-        <v>-1</v>
+        <f>1*6+1*5+3*4+2*2</f>
+        <v>27</v>
       </c>
       <c r="F17" s="5">
-        <v>-1</v>
+        <f>2*7+5*1</f>
+        <v>19</v>
       </c>
       <c r="G17" s="5">
-        <v>-1</v>
+        <f>1*5+1*4+2*3+3*2</f>
+        <v>21</v>
       </c>
       <c r="H17" s="5">
-        <v>-1</v>
+        <f>4*6+1*4+2*2</f>
+        <v>32</v>
       </c>
       <c r="I17" s="5">
-        <v>-1</v>
+        <f>3*7+1*6+1*5+2*4</f>
+        <v>40</v>
       </c>
       <c r="J17" s="5">
-        <v>-1</v>
+        <f>1*7+1*6+3*5+2*1</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D20" s="15"/>
+      <c r="E20" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D21" s="9"/>
+      <c r="E21" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D22" s="10"/>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D23" s="11"/>
+      <c r="E23" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D24" s="12"/>
+      <c r="E24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D25" s="13"/>
+      <c r="E25" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D26" s="14"/>
+      <c r="E26" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>